<commit_message>
Correct variable type, column sizes
CreateTsXPT.R now also needs write.xport2.R to correct the variable sizes as the package SASxport uses minimum column sizes of 8.
</commit_message>
<xml_diff>
--- a/contributed/Nonclinical/R/CreatingXPT/CreateTsXPT_StudyData.xlsx
+++ b/contributed/Nonclinical/R/CreatingXPT/CreateTsXPT_StudyData.xlsx
@@ -54,9 +54,6 @@
     <t>STITLE</t>
   </si>
   <si>
-    <t>Title</t>
-  </si>
-  <si>
     <t>STSTDTC</t>
   </si>
   <si>
@@ -139,6 +136,9 @@
   </si>
   <si>
     <t>Parameter Value</t>
+  </si>
+  <si>
+    <t>Study Title</t>
   </si>
 </sst>
 </file>
@@ -477,7 +477,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -489,7 +491,7 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
         <v>0</v>
@@ -512,53 +514,53 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
       <c r="D2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
         <v>34</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>35</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>36</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>37</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>38</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>39</v>
-      </c>
-      <c r="G3" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -570,15 +572,15 @@
         <v>7</v>
       </c>
       <c r="F4" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" t="s">
         <v>14</v>
-      </c>
-      <c r="G4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -598,7 +600,7 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -610,15 +612,15 @@
         <v>11</v>
       </c>
       <c r="F6" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="G6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -627,18 +629,18 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>6</v>
@@ -650,15 +652,15 @@
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:7">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
         <v>6</v>
@@ -673,12 +675,12 @@
         <v>9</v>
       </c>
       <c r="G9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:7">
       <c r="A10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>6</v>
@@ -690,15 +692,15 @@
         <v>11</v>
       </c>
       <c r="F10" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -707,18 +709,18 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -730,15 +732,15 @@
         <v>7</v>
       </c>
       <c r="F12" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="G12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -753,12 +755,12 @@
         <v>9</v>
       </c>
       <c r="G13" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -770,15 +772,15 @@
         <v>11</v>
       </c>
       <c r="F14" t="s">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="G14" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -787,33 +789,33 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F15" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
+        <v>31</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="20" spans="7:7">

</xml_diff>

<commit_message>
Added other desirable parameter codes to the example
</commit_message>
<xml_diff>
--- a/contributed/Nonclinical/R/CreatingXPT/CreateTsXPT_StudyData.xlsx
+++ b/contributed/Nonclinical/R/CreatingXPT/CreateTsXPT_StudyData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="52">
   <si>
     <t>DOMAIN</t>
   </si>
@@ -66,9 +66,6 @@
     <t>STUDYID</t>
   </si>
   <si>
-    <t>Example of a 4-week Repeat-Dose Toxicity Study in Rats with a 1-week Recovery</t>
-  </si>
-  <si>
     <t>Study Start Date</t>
   </si>
   <si>
@@ -139,15 +136,48 @@
   </si>
   <si>
     <t>Study Title</t>
+  </si>
+  <si>
+    <t>SSPONSOR</t>
+  </si>
+  <si>
+    <t>TRT</t>
+  </si>
+  <si>
+    <t>DOSDUR</t>
+  </si>
+  <si>
+    <t>TRTCAS</t>
+  </si>
+  <si>
+    <t>Sponsoring Organization</t>
+  </si>
+  <si>
+    <t>Example Sponsor Inc.</t>
+  </si>
+  <si>
+    <t>Example Compound Name</t>
+  </si>
+  <si>
+    <t>Investigational Therapy or Treatment</t>
+  </si>
+  <si>
+    <t>Dosing Duration</t>
+  </si>
+  <si>
+    <t>P28D</t>
+  </si>
+  <si>
+    <t>Primary Treatment CAS Registry Number</t>
+  </si>
+  <si>
+    <t>58-08-2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-  </numFmts>
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -177,10 +207,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -475,16 +504,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G26"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
+    <col min="2" max="2" width="19.88671875" customWidth="1"/>
     <col min="5" max="5" width="13.88671875" customWidth="1"/>
-    <col min="6" max="6" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="35.6640625" customWidth="1"/>
     <col min="7" max="7" width="65.44140625" customWidth="1"/>
     <col min="9" max="9" width="8.88671875" customWidth="1"/>
   </cols>
@@ -514,53 +542,53 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2" t="s">
         <v>18</v>
       </c>
-      <c r="B2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" t="s">
-        <v>19</v>
-      </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" t="s">
         <v>33</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>34</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>35</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>36</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>37</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>38</v>
-      </c>
-      <c r="G3" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="4" spans="1:7">
       <c r="A4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
         <v>6</v>
@@ -569,18 +597,18 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="F4" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="G4" t="s">
-        <v>14</v>
+        <v>45</v>
       </c>
     </row>
     <row r="5" spans="1:7">
       <c r="A5" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -589,18 +617,18 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>8</v>
+        <v>41</v>
       </c>
       <c r="F5" t="s">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="G5" t="s">
-        <v>10</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
@@ -609,18 +637,18 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>9</v>
       </c>
       <c r="G6" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
         <v>6</v>
@@ -629,13 +657,13 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>20</v>
+        <v>13</v>
+      </c>
+      <c r="G7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7">
@@ -649,13 +677,13 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>7</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:7">
@@ -669,13 +697,13 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="F9" t="s">
-        <v>9</v>
+        <v>50</v>
       </c>
       <c r="G9" t="s">
-        <v>22</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7">
@@ -689,18 +717,18 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
-      </c>
-      <c r="G10" t="s">
-        <v>28</v>
+        <v>16</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" t="s">
         <v>6</v>
@@ -709,18 +737,18 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F11" t="s">
-        <v>17</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>23</v>
+        <v>13</v>
+      </c>
+      <c r="G11" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B12" t="s">
         <v>6</v>
@@ -729,10 +757,10 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="F12" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="G12" t="s">
         <v>21</v>
@@ -740,7 +768,7 @@
     </row>
     <row r="13" spans="1:7">
       <c r="A13" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B13" t="s">
         <v>6</v>
@@ -749,10 +777,10 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>39</v>
       </c>
       <c r="G13" t="s">
         <v>27</v>
@@ -760,7 +788,7 @@
     </row>
     <row r="14" spans="1:7">
       <c r="A14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B14" t="s">
         <v>6</v>
@@ -769,18 +797,18 @@
         <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="F14" t="s">
-        <v>40</v>
-      </c>
-      <c r="G14" t="s">
-        <v>29</v>
+        <v>16</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B15" t="s">
         <v>6</v>
@@ -789,56 +817,99 @@
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="F15" t="s">
-        <v>17</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
+      </c>
+      <c r="G15" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="A16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B16" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>8</v>
+      </c>
+      <c r="F16" t="s">
+        <v>9</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B17" t="s">
+        <v>6</v>
+      </c>
+      <c r="C17">
+        <v>1</v>
+      </c>
+      <c r="E17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18" t="s">
+        <v>6</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" t="s">
+        <v>16</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="E19" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" t="s">
+        <v>16</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B16" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="E16" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" t="s">
-        <v>17</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="20" spans="7:7">
-      <c r="G20" s="2"/>
-    </row>
-    <row r="21" spans="7:7">
-      <c r="G21" s="2"/>
-    </row>
-    <row r="23" spans="7:7">
-      <c r="G23" s="2"/>
-    </row>
-    <row r="24" spans="7:7">
-      <c r="G24" s="2"/>
-    </row>
-    <row r="25" spans="7:7">
-      <c r="G25" s="2"/>
-    </row>
-    <row r="26" spans="7:7">
-      <c r="G26" s="2"/>
     </row>
   </sheetData>
   <dataConsolidate/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>